<commit_message>
Update spreadsheets to use CExxx instead of Exxx for test case names
</commit_message>
<xml_diff>
--- a/input/CodyRun/1/Std140_CE_b_Output.xlsx
+++ b/input/CodyRun/1/Std140_CE_b_Output.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\JasonGlazer--ashrae-140-automation\input\CodyRun\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{246AB832-14F5-4A8D-8118-7F1288BE944F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5D6735-FB03-4FDA-AB7A-7A311E29A4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24945" yWindow="2670" windowWidth="30675" windowHeight="17970" xr2:uid="{3967BC36-3351-4A62-97C9-7FE3A6239BBD}"/>
+    <workbookView xWindow="3570" yWindow="660" windowWidth="33600" windowHeight="20790" xr2:uid="{3967BC36-3351-4A62-97C9-7FE3A6239BBD}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_Fill" hidden="1">#REF!</definedName>
   </definedNames>
@@ -251,12 +248,6 @@
     <t xml:space="preserve">   A n n u a l   H o u r l y   I n t e g r a t e d   M a x i m a   C o n s u m p t i o n s   a n d   L o a d s</t>
   </si>
   <si>
-    <t xml:space="preserve">         E300 Only, Maxima</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  E 3 0 0   O n l y</t>
-  </si>
-  <si>
     <t>Zone</t>
   </si>
   <si>
@@ -348,78 +339,6 @@
   </si>
   <si>
     <t>kg/kg</t>
-  </si>
-  <si>
-    <t>E300</t>
-  </si>
-  <si>
-    <t>E310</t>
-  </si>
-  <si>
-    <t>E320</t>
-  </si>
-  <si>
-    <t>E330</t>
-  </si>
-  <si>
-    <t>E340</t>
-  </si>
-  <si>
-    <t>E350</t>
-  </si>
-  <si>
-    <t>E360</t>
-  </si>
-  <si>
-    <t>E400</t>
-  </si>
-  <si>
-    <t>E410</t>
-  </si>
-  <si>
-    <t>E420</t>
-  </si>
-  <si>
-    <t>E430</t>
-  </si>
-  <si>
-    <t>E440</t>
-  </si>
-  <si>
-    <t>E500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E500 </t>
-  </si>
-  <si>
-    <t>E500 May-Sep</t>
-  </si>
-  <si>
-    <t>E510</t>
-  </si>
-  <si>
-    <t>E510 May-Sep</t>
-  </si>
-  <si>
-    <t>E520</t>
-  </si>
-  <si>
-    <t>E522</t>
-  </si>
-  <si>
-    <t>E525</t>
-  </si>
-  <si>
-    <t>E530</t>
-  </si>
-  <si>
-    <t>E540</t>
-  </si>
-  <si>
-    <t>E545</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> J u n e   2 8   H o u r l y   O u t p u t   -   C a s e   E 3 0 0</t>
   </si>
   <si>
     <t xml:space="preserve">             A n n u a l   H o u r l y   I n t e g r a t e d   M a x i m a   a n d   M i n i m a   -   C O P 2   a n d   Z o n e</t>
@@ -566,9 +485,6 @@
     <t>24</t>
   </si>
   <si>
-    <t xml:space="preserve">      C a s e   E 5 0 0   A v e r a g e   D a i l y   O u t p u t s  -  f(ODB) sensitivity</t>
-  </si>
-  <si>
     <t xml:space="preserve">   Evaporator Coil Load</t>
   </si>
   <si>
@@ -584,7 +500,88 @@
     <t>June 25</t>
   </si>
   <si>
-    <t xml:space="preserve">      C a s e   E 5 3 0   A v e r a g e   D a i l y   O u t p u t s  -  f(ODB) sensitivity</t>
+    <t>CE300</t>
+  </si>
+  <si>
+    <t>CE310</t>
+  </si>
+  <si>
+    <t>CE320</t>
+  </si>
+  <si>
+    <t>CE330</t>
+  </si>
+  <si>
+    <t>CE340</t>
+  </si>
+  <si>
+    <t>CE350</t>
+  </si>
+  <si>
+    <t>CE360</t>
+  </si>
+  <si>
+    <t>CE400</t>
+  </si>
+  <si>
+    <t>CE410</t>
+  </si>
+  <si>
+    <t>CE420</t>
+  </si>
+  <si>
+    <t>CE430</t>
+  </si>
+  <si>
+    <t>CE440</t>
+  </si>
+  <si>
+    <t>CE500</t>
+  </si>
+  <si>
+    <t>CE500 May-SCEp</t>
+  </si>
+  <si>
+    <t>CE510 May-SCEp</t>
+  </si>
+  <si>
+    <t>CE520</t>
+  </si>
+  <si>
+    <t>CE522</t>
+  </si>
+  <si>
+    <t>CE525</t>
+  </si>
+  <si>
+    <t>CE530</t>
+  </si>
+  <si>
+    <t>CE540</t>
+  </si>
+  <si>
+    <t>CE545</t>
+  </si>
+  <si>
+    <t>C E 3 0 0   O n l y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE500 </t>
+  </si>
+  <si>
+    <t>CE510</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         CE300 Only, Maxima</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> J u n e   2 8   H o u r l y   O u t p u t   -   C a s e   C E 3 0 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      C a s e   C E 5 0 0   A v e r a g e   D a i l y   O u t p u t s  -  f(ODB) sensitivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      C a s e   C E 5 3 0   A v e r a g e   D a i l y   O u t p u t s  -  f(ODB) sensitivity</t>
   </si>
 </sst>
 </file>
@@ -1176,6 +1173,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1185,8 +1184,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1203,116 +1200,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Read Me"/>
-      <sheetName val="Adding Results"/>
-      <sheetName val="YourData"/>
-      <sheetName val="Title Page"/>
-      <sheetName val="Program List"/>
-      <sheetName val="Tables List"/>
-      <sheetName val="Figures List"/>
-      <sheetName val="Table-Q"/>
-      <sheetName val="Table-R"/>
-      <sheetName val="Table-S"/>
-      <sheetName val="Table-T"/>
-      <sheetName val="Fig B16.5.2-1 Qtot"/>
-      <sheetName val="Fig B16.5.2-2 dQtot"/>
-      <sheetName val="Fig B16.5.2-3 Ptot"/>
-      <sheetName val="Fig B16.5.2-4 dPtot"/>
-      <sheetName val="Fig B16.5.2-5 Qcomp"/>
-      <sheetName val="Fig B16.5.2-6 dQcomp"/>
-      <sheetName val="Fig B16.5.2-7 Qidfan"/>
-      <sheetName val="Fig B16.5.2-8 dQidfan"/>
-      <sheetName val="Fig B16.5.2-9 Qodfan"/>
-      <sheetName val="Fig B16.5.2-10 dQodfan"/>
-      <sheetName val="Fig B16.5.2-11 QCtot"/>
-      <sheetName val="Fig B16.5.2-12 PCtot"/>
-      <sheetName val="Fig B16.5.2-13 dPCtot"/>
-      <sheetName val="Fig B16.5.2-14 QCSens"/>
-      <sheetName val="Fig B16.5.2-15 dQCsens"/>
-      <sheetName val="Fig B16.5.2-16 PCSens"/>
-      <sheetName val="Fig B16.5.2-17 QClat"/>
-      <sheetName val="Fig B16.5.2-18 dQClat"/>
-      <sheetName val="Fig B16.5.2-19 PClat"/>
-      <sheetName val="Fig B16.5.2-20 dPClat"/>
-      <sheetName val="Fig B16.5.2-21 COP2"/>
-      <sheetName val="Fig B16.5.2-22 dCOP2"/>
-      <sheetName val="Fig B16.5.2-23 MxCOP2"/>
-      <sheetName val="Fig B16.5.2-24 dMxCOP2"/>
-      <sheetName val="Fig B16.5.2-25 MnCOP2"/>
-      <sheetName val="Fig B16.5.2-26 dMnCOP2"/>
-      <sheetName val="Fig B16.5.2-27 IDB"/>
-      <sheetName val="Fig B16.5.2-28 dIDB"/>
-      <sheetName val="Fig B16.5.2-29 MxIDB"/>
-      <sheetName val="Fig B16.5.2-30 dMxIDB"/>
-      <sheetName val="Fig B16.5.2-31 MnIDB"/>
-      <sheetName val="Fig B16.5.2-32 Humrat"/>
-      <sheetName val="Fig B16.5.2-33 dHumrat"/>
-      <sheetName val="Fig B16.5.2-34 MxHum"/>
-      <sheetName val="Fig B16.5.2-35 dMxHumrat"/>
-      <sheetName val="Fig B16.5.2-36 MnHum"/>
-      <sheetName val="Fig B16.5.2-37 RelHum"/>
-      <sheetName val="Fig B16.5.2-38 dRelHum"/>
-      <sheetName val="Fig B16.5.2-39 MxRelHum"/>
-      <sheetName val="Fig B16.5.2-40 dMxRelHum"/>
-      <sheetName val="Fig B16.5.2-41 MnRelHum"/>
-      <sheetName val="Fig B16.5.2-42 Qf(ODB)"/>
-      <sheetName val="Fig B16.5.2-43 QCf(ODB)"/>
-      <sheetName val="Fig B16.5.2-44 COP2f(ODB)"/>
-      <sheetName val="Fig B16.5.2-45 Humratf(ODB)"/>
-      <sheetName val="Fig B16.5.2-46 HrQ"/>
-      <sheetName val="Fig B16.5.2-47 HrQC"/>
-      <sheetName val="Fig B16.5.2-48 HrCOP2"/>
-      <sheetName val="Fig B16.5.2-49 HrHum"/>
-      <sheetName val="Fig B16.5.2-50 HrEDB,EWB"/>
-      <sheetName val="Fig B16.5.2-51 HrODB"/>
-      <sheetName val="Fig B16.5.2-52 HrOHR"/>
-      <sheetName val="A"/>
-      <sheetName val="Qdata"/>
-      <sheetName val="Rdata"/>
-      <sheetName val="Sdata"/>
-      <sheetName val="Tdata"/>
-      <sheetName val="TRNSYS-TUD"/>
-      <sheetName val="DOE22"/>
-      <sheetName val="DOE21E"/>
-      <sheetName val="EnergyPlus1.0"/>
-      <sheetName val="CodyRun"/>
-      <sheetName val="HOT3000"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="63"/>
-      <sheetData sheetId="64"/>
-      <sheetData sheetId="65"/>
-      <sheetData sheetId="66"/>
-      <sheetData sheetId="67"/>
-      <sheetData sheetId="68"/>
-      <sheetData sheetId="69"/>
-      <sheetData sheetId="70"/>
-      <sheetData sheetId="71"/>
-      <sheetData sheetId="72"/>
-      <sheetData sheetId="73"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1638,7 +1525,7 @@
   <dimension ref="A1:AR130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="L138" sqref="L138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1977,7 +1864,7 @@
       <c r="AB56" s="8"/>
       <c r="AC56" s="11"/>
       <c r="AD56" s="11" t="s">
-        <v>69</v>
+        <v>174</v>
       </c>
       <c r="AE56" s="11"/>
       <c r="AF56" s="11"/>
@@ -1998,7 +1885,7 @@
       <c r="K57" s="15"/>
       <c r="L57" s="16"/>
       <c r="M57" s="17" t="s">
-        <v>70</v>
+        <v>171</v>
       </c>
       <c r="N57" s="18"/>
       <c r="P57" s="13"/>
@@ -2033,14 +1920,14 @@
       <c r="I58" s="6"/>
       <c r="J58" s="7"/>
       <c r="K58" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L58" s="22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M58" s="23"/>
       <c r="N58" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O58" s="2"/>
       <c r="P58" s="13"/>
@@ -2057,47 +1944,47 @@
       <c r="AA58" s="7"/>
       <c r="AB58" s="8"/>
       <c r="AD58" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AH58" s="12"/>
     </row>
     <row r="59" spans="1:34">
       <c r="A59" s="13"/>
       <c r="B59" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C59" s="23"/>
       <c r="D59" s="23"/>
       <c r="E59" s="26"/>
       <c r="F59" s="25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G59" s="23"/>
       <c r="H59" s="26"/>
       <c r="I59" s="25"/>
       <c r="J59" s="23"/>
       <c r="K59" s="27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L59" s="28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M59" s="23"/>
       <c r="N59" s="24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O59" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P59" s="13"/>
       <c r="R59" s="29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S59" s="26"/>
       <c r="T59" s="25"/>
       <c r="U59" s="23"/>
       <c r="V59" s="23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="X59" s="23"/>
       <c r="Y59" s="23"/>
@@ -2109,126 +1996,126 @@
     </row>
     <row r="60" spans="1:34">
       <c r="A60" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B60" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C60" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="B60" s="31" t="s">
+      <c r="D60" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C60" s="27" t="s">
+      <c r="E60" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="D60" s="27" t="s">
+      <c r="F60" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="G60" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="E60" s="28" t="s">
+      <c r="H60" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="F60" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="G60" s="27" t="s">
+      <c r="I60" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="H60" s="28" t="s">
+      <c r="J60" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="I60" s="31" t="s">
+      <c r="K60" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="J60" s="27" t="s">
+      <c r="L60" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="M60" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="K60" s="27" t="s">
+      <c r="N60" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="O60" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="P60" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="R60" s="29" t="s">
         <v>89</v>
-      </c>
-      <c r="L60" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="M60" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="N60" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="O60" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="P60" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="R60" s="29" t="s">
-        <v>91</v>
       </c>
       <c r="S60" s="26"/>
       <c r="T60" s="25"/>
       <c r="U60" s="27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="V60" s="23"/>
       <c r="W60" s="32"/>
       <c r="X60" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Y60" s="23"/>
       <c r="Z60" s="32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AA60" s="23"/>
       <c r="AB60" s="26"/>
       <c r="AD60" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AE60" s="30"/>
       <c r="AF60" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AH60" s="30"/>
     </row>
     <row r="61" spans="1:34">
       <c r="A61" s="33"/>
       <c r="B61" s="34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C61" s="35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D61" s="35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E61" s="36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F61" s="34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G61" s="35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H61" s="36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I61" s="14"/>
       <c r="J61" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="K61" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="L61" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="K61" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="L61" s="36" t="s">
-        <v>98</v>
-      </c>
       <c r="M61" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="N61" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="O61" s="39" t="s">
         <v>96</v>
-      </c>
-      <c r="N61" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="O61" s="39" t="s">
-        <v>98</v>
       </c>
       <c r="P61" s="40"/>
       <c r="Q61" s="34" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="R61" s="35" t="s">
         <v>62</v>
@@ -2237,7 +2124,7 @@
         <v>63</v>
       </c>
       <c r="T61" s="34" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="U61" s="35" t="s">
         <v>62</v>
@@ -2246,7 +2133,7 @@
         <v>63</v>
       </c>
       <c r="W61" s="41" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="X61" s="35" t="s">
         <v>62</v>
@@ -2255,7 +2142,7 @@
         <v>63</v>
       </c>
       <c r="Z61" s="41" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AA61" s="35" t="s">
         <v>62</v>
@@ -2264,7 +2151,7 @@
         <v>63</v>
       </c>
       <c r="AC61" s="39" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AD61" s="39" t="s">
         <v>62</v>
@@ -2273,7 +2160,7 @@
         <v>63</v>
       </c>
       <c r="AF61" s="39" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AG61" s="39" t="s">
         <v>62</v>
@@ -2284,7 +2171,7 @@
     </row>
     <row r="62" spans="1:34" ht="15.75">
       <c r="A62" s="13" t="s">
-        <v>102</v>
+        <v>150</v>
       </c>
       <c r="B62" s="43">
         <v>34976.411000001252</v>
@@ -2330,7 +2217,7 @@
         <v>0.47826141552511653</v>
       </c>
       <c r="P62" s="5" t="s">
-        <v>102</v>
+        <v>150</v>
       </c>
       <c r="Q62" s="43">
         <v>11932</v>
@@ -2389,7 +2276,7 @@
     </row>
     <row r="63" spans="1:34" ht="15.75">
       <c r="A63" s="13" t="s">
-        <v>103</v>
+        <v>151</v>
       </c>
       <c r="B63" s="53">
         <v>39519.569000001269</v>
@@ -2431,7 +2318,7 @@
         <v>0.57840981735158392</v>
       </c>
       <c r="P63" s="13" t="s">
-        <v>103</v>
+        <v>151</v>
       </c>
       <c r="Q63" s="53">
         <v>12653</v>
@@ -2474,7 +2361,7 @@
     </row>
     <row r="64" spans="1:34" ht="15.75">
       <c r="A64" s="13" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="B64" s="53">
         <v>39400.815000001385</v>
@@ -2516,7 +2403,7 @@
         <v>0.51103424657534458</v>
       </c>
       <c r="P64" s="13" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="Q64" s="53">
         <v>13104</v>
@@ -2559,7 +2446,7 @@
     </row>
     <row r="65" spans="1:34" ht="15.75">
       <c r="A65" s="13" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="B65" s="53">
         <v>40535.137000001225</v>
@@ -2601,7 +2488,7 @@
         <v>0.50084817351598265</v>
       </c>
       <c r="P65" s="13" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="Q65" s="53">
         <v>13467</v>
@@ -2644,7 +2531,7 @@
     </row>
     <row r="66" spans="1:34" ht="15.75">
       <c r="A66" s="13" t="s">
-        <v>106</v>
+        <v>154</v>
       </c>
       <c r="B66" s="53">
         <v>40065.261000001236</v>
@@ -2686,7 +2573,7 @@
         <v>0.50296689497717151</v>
       </c>
       <c r="P66" s="13" t="s">
-        <v>106</v>
+        <v>154</v>
       </c>
       <c r="Q66" s="53">
         <v>13277</v>
@@ -2733,7 +2620,7 @@
     </row>
     <row r="67" spans="1:34" ht="15.75">
       <c r="A67" s="13" t="s">
-        <v>107</v>
+        <v>155</v>
       </c>
       <c r="B67" s="53">
         <v>31586.592000001216</v>
@@ -2775,7 +2662,7 @@
         <v>0.44316210045662174</v>
       </c>
       <c r="P67" s="13" t="s">
-        <v>107</v>
+        <v>155</v>
       </c>
       <c r="Q67" s="53">
         <v>11932</v>
@@ -2818,7 +2705,7 @@
     </row>
     <row r="68" spans="1:34" ht="15.75">
       <c r="A68" s="40" t="s">
-        <v>108</v>
+        <v>156</v>
       </c>
       <c r="B68" s="60">
         <v>54843.258000001253</v>
@@ -2860,7 +2747,7 @@
         <v>0.40871004566211877</v>
       </c>
       <c r="P68" s="40" t="s">
-        <v>108</v>
+        <v>156</v>
       </c>
       <c r="Q68" s="60">
         <v>12863</v>
@@ -2903,7 +2790,7 @@
     </row>
     <row r="69" spans="1:34" ht="15.75">
       <c r="A69" s="32" t="s">
-        <v>109</v>
+        <v>157</v>
       </c>
       <c r="B69" s="65"/>
       <c r="C69" s="66"/>
@@ -2920,7 +2807,7 @@
       <c r="N69" s="57"/>
       <c r="O69" s="57"/>
       <c r="P69" s="32" t="s">
-        <v>109</v>
+        <v>157</v>
       </c>
       <c r="Q69" s="65"/>
       <c r="R69" s="66"/>
@@ -2939,7 +2826,7 @@
     </row>
     <row r="70" spans="1:34" ht="15.75">
       <c r="A70" s="32" t="s">
-        <v>110</v>
+        <v>158</v>
       </c>
       <c r="B70" s="65"/>
       <c r="C70" s="66"/>
@@ -2956,7 +2843,7 @@
       <c r="N70" s="57"/>
       <c r="O70" s="57"/>
       <c r="P70" s="32" t="s">
-        <v>110</v>
+        <v>158</v>
       </c>
       <c r="Q70" s="65"/>
       <c r="R70" s="66"/>
@@ -2975,7 +2862,7 @@
     </row>
     <row r="71" spans="1:34" ht="15.75">
       <c r="A71" s="32" t="s">
-        <v>111</v>
+        <v>159</v>
       </c>
       <c r="B71" s="65"/>
       <c r="C71" s="66"/>
@@ -2992,7 +2879,7 @@
       <c r="N71" s="57"/>
       <c r="O71" s="57"/>
       <c r="P71" s="32" t="s">
-        <v>111</v>
+        <v>159</v>
       </c>
       <c r="Q71" s="65"/>
       <c r="R71" s="66"/>
@@ -3011,7 +2898,7 @@
     </row>
     <row r="72" spans="1:34" ht="15.75">
       <c r="A72" s="32" t="s">
-        <v>112</v>
+        <v>160</v>
       </c>
       <c r="B72" s="65"/>
       <c r="C72" s="66"/>
@@ -3028,7 +2915,7 @@
       <c r="N72" s="57"/>
       <c r="O72" s="57"/>
       <c r="P72" s="32" t="s">
-        <v>112</v>
+        <v>160</v>
       </c>
       <c r="Q72" s="65"/>
       <c r="R72" s="66"/>
@@ -3047,7 +2934,7 @@
     </row>
     <row r="73" spans="1:34" ht="15.75">
       <c r="A73" s="32" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="B73" s="65"/>
       <c r="C73" s="66"/>
@@ -3064,7 +2951,7 @@
       <c r="N73" s="57"/>
       <c r="O73" s="57"/>
       <c r="P73" s="32" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="Q73" s="65"/>
       <c r="R73" s="66"/>
@@ -3083,7 +2970,7 @@
     </row>
     <row r="74" spans="1:34" ht="15.75">
       <c r="A74" s="5" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="B74" s="43">
         <v>22322.953000000023</v>
@@ -3125,7 +3012,7 @@
         <v>0.659418949771712</v>
       </c>
       <c r="P74" s="5" t="s">
-        <v>115</v>
+        <v>172</v>
       </c>
       <c r="Q74" s="43">
         <v>10177</v>
@@ -3168,7 +3055,7 @@
     </row>
     <row r="75" spans="1:34" ht="15.75">
       <c r="A75" s="13" t="s">
-        <v>116</v>
+        <v>163</v>
       </c>
       <c r="B75" s="53">
         <v>17434.537000000029</v>
@@ -3210,7 +3097,7 @@
         <v>0.5707216775598879</v>
       </c>
       <c r="P75" s="13" t="s">
-        <v>117</v>
+        <v>173</v>
       </c>
       <c r="Q75" s="53">
         <v>11186</v>
@@ -3253,7 +3140,7 @@
     </row>
     <row r="76" spans="1:34" ht="15.75">
       <c r="A76" s="13" t="s">
-        <v>118</v>
+        <v>164</v>
       </c>
       <c r="B76" s="53">
         <v>34848.63700000001</v>
@@ -3295,7 +3182,7 @@
         <v>0.57061546840956057</v>
       </c>
       <c r="P76" s="13" t="s">
-        <v>119</v>
+        <v>165</v>
       </c>
       <c r="Q76" s="53">
         <v>11044</v>
@@ -3338,7 +3225,7 @@
     </row>
     <row r="77" spans="1:34" ht="15.75">
       <c r="A77" s="13" t="s">
-        <v>119</v>
+        <v>165</v>
       </c>
       <c r="B77" s="53">
         <v>25131.070000000262</v>
@@ -3380,7 +3267,7 @@
         <v>0.70226826484016935</v>
       </c>
       <c r="P77" s="13" t="s">
-        <v>120</v>
+        <v>166</v>
       </c>
       <c r="Q77" s="53">
         <v>10639</v>
@@ -3423,7 +3310,7 @@
     </row>
     <row r="78" spans="1:34" ht="15.75">
       <c r="A78" s="13" t="s">
-        <v>120</v>
+        <v>166</v>
       </c>
       <c r="B78" s="53">
         <v>23619.743999999955</v>
@@ -3465,7 +3352,7 @@
         <v>0.68231392694061999</v>
       </c>
       <c r="P78" s="13" t="s">
-        <v>121</v>
+        <v>167</v>
       </c>
       <c r="Q78" s="53">
         <v>9419</v>
@@ -3508,7 +3395,7 @@
     </row>
     <row r="79" spans="1:34" ht="15.75">
       <c r="A79" s="13" t="s">
-        <v>121</v>
+        <v>167</v>
       </c>
       <c r="B79" s="53">
         <v>20241.712999999996</v>
@@ -3550,7 +3437,7 @@
         <v>0.60138698630132004</v>
       </c>
       <c r="P79" s="13" t="s">
-        <v>122</v>
+        <v>168</v>
       </c>
       <c r="Q79" s="53">
         <v>7992</v>
@@ -3593,7 +3480,7 @@
     </row>
     <row r="80" spans="1:34" ht="15.75">
       <c r="A80" s="13" t="s">
-        <v>122</v>
+        <v>168</v>
       </c>
       <c r="B80" s="71">
         <v>17442.46800000007</v>
@@ -3635,7 +3522,7 @@
         <v>0.41451598173521698</v>
       </c>
       <c r="P80" s="13" t="s">
-        <v>123</v>
+        <v>169</v>
       </c>
       <c r="Q80" s="53">
         <v>8846</v>
@@ -3678,7 +3565,7 @@
     </row>
     <row r="81" spans="1:44" ht="15.75">
       <c r="A81" s="13" t="s">
-        <v>123</v>
+        <v>169</v>
       </c>
       <c r="B81" s="53">
         <v>19536.572000000106</v>
@@ -3720,7 +3607,7 @@
         <v>0.40050913242005715</v>
       </c>
       <c r="P81" s="40" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="Q81" s="60">
         <v>7351</v>
@@ -3763,7 +3650,7 @@
     </row>
     <row r="82" spans="1:44" ht="15.75">
       <c r="A82" s="40" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="B82" s="60">
         <v>15791.080999999982</v>
@@ -3811,7 +3698,7 @@
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
       <c r="E84" s="7" t="s">
-        <v>125</v>
+        <v>175</v>
       </c>
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
@@ -3825,7 +3712,7 @@
       <c r="R84" s="9"/>
       <c r="S84" s="9"/>
       <c r="T84" s="9" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="U84" s="9"/>
       <c r="V84" s="9"/>
@@ -3892,36 +3779,36 @@
     <row r="86" spans="1:44" ht="15.75">
       <c r="A86" s="13"/>
       <c r="B86" s="6" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="C86" s="8"/>
       <c r="D86" s="6" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="E86" s="7"/>
       <c r="F86" s="8"/>
       <c r="G86" s="76" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H86" s="5"/>
       <c r="I86" s="6"/>
       <c r="J86" s="7"/>
       <c r="K86" s="8"/>
       <c r="L86" s="76" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="P86" s="13"/>
       <c r="Q86" s="23"/>
       <c r="R86" s="23"/>
       <c r="S86" s="23" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="T86" s="23"/>
       <c r="U86" s="23"/>
       <c r="V86" s="23"/>
       <c r="W86" s="32"/>
       <c r="X86" s="23" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="Y86" s="23"/>
       <c r="Z86" s="23"/>
@@ -3929,7 +3816,7 @@
       <c r="AB86" s="23"/>
       <c r="AC86" s="32"/>
       <c r="AD86" s="23" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="AE86" s="23"/>
       <c r="AF86" s="23"/>
@@ -3937,7 +3824,7 @@
       <c r="AH86" s="23"/>
       <c r="AI86" s="32"/>
       <c r="AJ86" s="23" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="AK86" s="23"/>
       <c r="AL86" s="23"/>
@@ -3950,79 +3837,79 @@
         <v>63</v>
       </c>
       <c r="B87" s="31" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C87" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D87" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E87" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="D87" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="E87" s="27" t="s">
-        <v>85</v>
-      </c>
       <c r="F87" s="28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G87" s="78" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="H87" s="78" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="I87" s="31" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J87" s="27" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="K87" s="28" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="L87" s="78" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="P87" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q87" s="23"/>
       <c r="R87" s="23" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="S87" s="23"/>
       <c r="T87" s="32"/>
       <c r="U87" s="23" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="V87" s="23"/>
       <c r="W87" s="32"/>
       <c r="X87" s="23" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="Y87" s="23"/>
       <c r="Z87" s="32"/>
       <c r="AA87" s="23" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="AB87" s="23"/>
       <c r="AC87" s="32"/>
       <c r="AD87" s="23" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="AE87" s="23"/>
       <c r="AF87" s="32"/>
       <c r="AG87" s="23" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="AH87" s="23"/>
       <c r="AI87" s="32"/>
       <c r="AJ87" s="23" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="AK87" s="23"/>
       <c r="AL87" s="32"/>
       <c r="AM87" s="23" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="AN87" s="77"/>
       <c r="AR87" s="75"/>
@@ -4030,39 +3917,39 @@
     <row r="88" spans="1:44" ht="15.75">
       <c r="A88" s="40"/>
       <c r="B88" s="34" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="C88" s="36" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="D88" s="34" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="E88" s="35" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="F88" s="36" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="G88" s="79" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="H88" s="40"/>
       <c r="I88" s="34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J88" s="35" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K88" s="36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L88" s="79" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="P88" s="40"/>
       <c r="Q88" s="27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="R88" s="27" t="s">
         <v>62</v>
@@ -4071,7 +3958,7 @@
         <v>63</v>
       </c>
       <c r="T88" s="80" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="U88" s="27" t="s">
         <v>62</v>
@@ -4080,7 +3967,7 @@
         <v>63</v>
       </c>
       <c r="W88" s="80" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="X88" s="27" t="s">
         <v>62</v>
@@ -4089,7 +3976,7 @@
         <v>63</v>
       </c>
       <c r="Z88" s="80" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AA88" s="27" t="s">
         <v>62</v>
@@ -4098,7 +3985,7 @@
         <v>63</v>
       </c>
       <c r="AC88" s="81" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AD88" s="37" t="s">
         <v>62</v>
@@ -4107,7 +3994,7 @@
         <v>63</v>
       </c>
       <c r="AF88" s="81" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AG88" s="37" t="s">
         <v>62</v>
@@ -4116,7 +4003,7 @@
         <v>63</v>
       </c>
       <c r="AI88" s="81" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="AJ88" s="37" t="s">
         <v>62</v>
@@ -4125,7 +4012,7 @@
         <v>63</v>
       </c>
       <c r="AL88" s="81" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="AM88" s="37" t="s">
         <v>62</v>
@@ -4134,16 +4021,16 @@
         <v>63</v>
       </c>
       <c r="AO88" s="2" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="AP88" s="2" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="AR88" s="75"/>
     </row>
     <row r="89" spans="1:44" ht="15.75">
       <c r="A89" s="5" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="B89" s="43">
         <v>1886</v>
@@ -4179,7 +4066,7 @@
         <v>1.11E-2</v>
       </c>
       <c r="P89" s="5" t="s">
-        <v>102</v>
+        <v>150</v>
       </c>
       <c r="Q89" s="43">
         <v>3.8706106870229005</v>
@@ -4260,7 +4147,7 @@
     </row>
     <row r="90" spans="1:44" ht="15.75">
       <c r="A90" s="13" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="B90" s="53">
         <v>1964</v>
@@ -4296,7 +4183,7 @@
         <v>1.1462E-2</v>
       </c>
       <c r="P90" s="13" t="s">
-        <v>103</v>
+        <v>151</v>
       </c>
       <c r="Q90" s="53">
         <v>4.1276400367309449</v>
@@ -4377,7 +4264,7 @@
     </row>
     <row r="91" spans="1:44" ht="15.75">
       <c r="A91" s="13" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="B91" s="53">
         <v>1881</v>
@@ -4413,7 +4300,7 @@
         <v>1.11E-2</v>
       </c>
       <c r="P91" s="13" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="Q91" s="53">
         <v>3.9433046993431025</v>
@@ -4494,7 +4381,7 @@
     </row>
     <row r="92" spans="1:44" ht="15.75">
       <c r="A92" s="13" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="B92" s="53">
         <v>1878</v>
@@ -4530,7 +4417,7 @@
         <v>1.11E-2</v>
       </c>
       <c r="P92" s="13" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="Q92" s="53">
         <v>4.1219461046450672</v>
@@ -4611,7 +4498,7 @@
     </row>
     <row r="93" spans="1:44" ht="15.75">
       <c r="A93" s="13" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="B93" s="53">
         <v>1756</v>
@@ -4647,7 +4534,7 @@
         <v>1.018E-2</v>
       </c>
       <c r="P93" s="13" t="s">
-        <v>106</v>
+        <v>154</v>
       </c>
       <c r="Q93" s="53">
         <v>4.0171608448415927</v>
@@ -4728,7 +4615,7 @@
     </row>
     <row r="94" spans="1:44" ht="15.75">
       <c r="A94" s="13" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="B94" s="53">
         <v>2075</v>
@@ -4764,7 +4651,7 @@
         <v>1.1001E-2</v>
       </c>
       <c r="P94" s="13" t="s">
-        <v>107</v>
+        <v>155</v>
       </c>
       <c r="Q94" s="53">
         <v>3.9320987654320994</v>
@@ -4845,7 +4732,7 @@
     </row>
     <row r="95" spans="1:44" ht="15.75">
       <c r="A95" s="13" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="B95" s="53">
         <v>3035</v>
@@ -4881,7 +4768,7 @@
         <v>1.3140000000000001E-2</v>
       </c>
       <c r="P95" s="40" t="s">
-        <v>108</v>
+        <v>156</v>
       </c>
       <c r="Q95" s="60">
         <v>4.4320100031259768</v>
@@ -4962,7 +4849,7 @@
     </row>
     <row r="96" spans="1:44" ht="15.75">
       <c r="A96" s="13" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
       <c r="B96" s="53">
         <v>3303</v>
@@ -4998,7 +4885,7 @@
         <v>1.1075E-2</v>
       </c>
       <c r="P96" s="32" t="s">
-        <v>109</v>
+        <v>157</v>
       </c>
       <c r="Q96" s="65"/>
       <c r="R96" s="66"/>
@@ -5030,7 +4917,7 @@
     </row>
     <row r="97" spans="1:44" ht="15.75">
       <c r="A97" s="13" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="B97" s="53">
         <v>4483</v>
@@ -5066,7 +4953,7 @@
         <v>1.1995E-2</v>
       </c>
       <c r="P97" s="32" t="s">
-        <v>110</v>
+        <v>158</v>
       </c>
       <c r="Q97" s="65"/>
       <c r="R97" s="66"/>
@@ -5098,7 +4985,7 @@
     </row>
     <row r="98" spans="1:44" ht="15.75">
       <c r="A98" s="13" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
       <c r="B98" s="53">
         <v>4594</v>
@@ -5134,7 +5021,7 @@
         <v>1.2760000000000001E-2</v>
       </c>
       <c r="P98" s="32" t="s">
-        <v>111</v>
+        <v>159</v>
       </c>
       <c r="Q98" s="65"/>
       <c r="R98" s="66"/>
@@ -5166,7 +5053,7 @@
     </row>
     <row r="99" spans="1:44" ht="15.75">
       <c r="A99" s="13" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="B99" s="53">
         <v>5238</v>
@@ -5202,7 +5089,7 @@
         <v>1.4808999999999999E-2</v>
       </c>
       <c r="P99" s="32" t="s">
-        <v>112</v>
+        <v>160</v>
       </c>
       <c r="Q99" s="65"/>
       <c r="R99" s="66"/>
@@ -5234,7 +5121,7 @@
     </row>
     <row r="100" spans="1:44" ht="15.75">
       <c r="A100" s="13" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="B100" s="53">
         <v>5066</v>
@@ -5270,7 +5157,7 @@
         <v>1.3252999999999999E-2</v>
       </c>
       <c r="P100" s="32" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="Q100" s="65"/>
       <c r="R100" s="66"/>
@@ -5302,7 +5189,7 @@
     </row>
     <row r="101" spans="1:44" ht="15.75">
       <c r="A101" s="13" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="B101" s="53">
         <v>6442</v>
@@ -5338,7 +5225,7 @@
         <v>1.1329000000000001E-2</v>
       </c>
       <c r="P101" s="5" t="s">
-        <v>115</v>
+        <v>172</v>
       </c>
       <c r="Q101" s="43">
         <v>4.1846218842416558</v>
@@ -5419,7 +5306,7 @@
     </row>
     <row r="102" spans="1:44" ht="15.75">
       <c r="A102" s="13" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
       <c r="B102" s="53">
         <v>6523</v>
@@ -5455,7 +5342,7 @@
         <v>1.1729E-2</v>
       </c>
       <c r="P102" s="13" t="s">
-        <v>117</v>
+        <v>173</v>
       </c>
       <c r="Q102" s="53">
         <v>4.6895843211632684</v>
@@ -5572,7 +5459,7 @@
         <v>1.2378999999999999E-2</v>
       </c>
       <c r="P103" s="13" t="s">
-        <v>119</v>
+        <v>165</v>
       </c>
       <c r="Q103" s="53">
         <v>3.8017291066282426</v>
@@ -5653,7 +5540,7 @@
     </row>
     <row r="104" spans="1:44" ht="15.75">
       <c r="A104" s="13" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="B104" s="53">
         <v>8169</v>
@@ -5689,7 +5576,7 @@
         <v>1.4232E-2</v>
       </c>
       <c r="P104" s="13" t="s">
-        <v>120</v>
+        <v>166</v>
       </c>
       <c r="Q104" s="53">
         <v>3.9857984589817197</v>
@@ -5769,7 +5656,7 @@
     </row>
     <row r="105" spans="1:44" ht="15.75">
       <c r="A105" s="13" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="B105" s="53">
         <v>5306</v>
@@ -5805,7 +5692,7 @@
         <v>1.473E-2</v>
       </c>
       <c r="P105" s="13" t="s">
-        <v>121</v>
+        <v>167</v>
       </c>
       <c r="Q105" s="53">
         <v>4.6380543633762521</v>
@@ -5885,7 +5772,7 @@
     </row>
     <row r="106" spans="1:44" ht="15.75">
       <c r="A106" s="13" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="B106" s="53">
         <v>5381</v>
@@ -5921,7 +5808,7 @@
         <v>1.5684E-2</v>
       </c>
       <c r="P106" s="13" t="s">
-        <v>122</v>
+        <v>168</v>
       </c>
       <c r="Q106" s="71">
         <v>3.8400447427293063</v>
@@ -6001,7 +5888,7 @@
     </row>
     <row r="107" spans="1:44" ht="15.75">
       <c r="A107" s="13" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="B107" s="53">
         <v>4791</v>
@@ -6037,7 +5924,7 @@
         <v>1.4539E-2</v>
       </c>
       <c r="P107" s="13" t="s">
-        <v>123</v>
+        <v>169</v>
       </c>
       <c r="Q107" s="71">
         <v>3.6666666666666665</v>
@@ -6117,7 +6004,7 @@
     </row>
     <row r="108" spans="1:44" ht="15.75">
       <c r="A108" s="13" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="B108" s="53">
         <v>4809</v>
@@ -6153,7 +6040,7 @@
         <v>1.6878000000000001E-2</v>
       </c>
       <c r="P108" s="40" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="Q108" s="103">
         <v>4.1564885496183201</v>
@@ -6233,7 +6120,7 @@
     </row>
     <row r="109" spans="1:44" ht="15.75">
       <c r="A109" s="13" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="B109" s="53">
         <v>3939</v>
@@ -6269,12 +6156,12 @@
         <v>1.6878000000000001E-2</v>
       </c>
       <c r="P109" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
     </row>
     <row r="110" spans="1:44" ht="15.75">
       <c r="A110" s="13" t="s">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="B110" s="53">
         <v>3852</v>
@@ -6313,7 +6200,7 @@
     </row>
     <row r="111" spans="1:44" ht="15.75">
       <c r="A111" s="13" t="s">
-        <v>169</v>
+        <v>143</v>
       </c>
       <c r="B111" s="53">
         <v>3752</v>
@@ -6351,7 +6238,7 @@
     </row>
     <row r="112" spans="1:44" ht="15.75">
       <c r="A112" s="40" t="s">
-        <v>170</v>
+        <v>144</v>
       </c>
       <c r="B112" s="60">
         <v>3794</v>
@@ -6390,7 +6277,7 @@
     <row r="115" spans="1:12">
       <c r="A115" s="5"/>
       <c r="B115" s="6" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
@@ -6419,19 +6306,19 @@
     </row>
     <row r="117" spans="1:12">
       <c r="A117" s="13"/>
-      <c r="B117" s="112" t="s">
-        <v>127</v>
-      </c>
-      <c r="C117" s="113"/>
-      <c r="D117" s="113"/>
-      <c r="E117" s="114"/>
+      <c r="B117" s="114" t="s">
+        <v>101</v>
+      </c>
+      <c r="C117" s="115"/>
+      <c r="D117" s="115"/>
+      <c r="E117" s="116"/>
       <c r="F117" s="6" t="s">
-        <v>172</v>
+        <v>145</v>
       </c>
       <c r="G117" s="7"/>
       <c r="H117" s="8"/>
       <c r="I117" s="76" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J117" s="5"/>
       <c r="K117" s="6"/>
@@ -6439,79 +6326,79 @@
     </row>
     <row r="118" spans="1:12">
       <c r="A118" s="13" t="s">
-        <v>173</v>
+        <v>146</v>
       </c>
       <c r="B118" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C118" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D118" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C118" s="27" t="s">
+      <c r="E118" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="D118" s="27" t="s">
+      <c r="F118" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="G118" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="E118" s="28" t="s">
+      <c r="H118" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="F118" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="G118" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="H118" s="28" t="s">
-        <v>86</v>
-      </c>
       <c r="I118" s="78" t="s">
-        <v>174</v>
+        <v>147</v>
       </c>
       <c r="J118" s="78" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="K118" s="31" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L118" s="28" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
     </row>
     <row r="119" spans="1:12">
       <c r="A119" s="40"/>
       <c r="B119" s="34" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="C119" s="35" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="D119" s="35" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="E119" s="36" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="F119" s="34" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="G119" s="35" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="H119" s="36" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="I119" s="79" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="J119" s="40"/>
       <c r="K119" s="34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L119" s="36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="120" spans="1:12" ht="15.75">
-      <c r="A120" s="115" t="s">
-        <v>175</v>
+      <c r="A120" s="112" t="s">
+        <v>148</v>
       </c>
       <c r="B120" s="43">
         <v>3901.0416666666665</v>
@@ -6548,8 +6435,8 @@
       </c>
     </row>
     <row r="121" spans="1:12" ht="15.75">
-      <c r="A121" s="116" t="s">
-        <v>176</v>
+      <c r="A121" s="113" t="s">
+        <v>149</v>
       </c>
       <c r="B121" s="60">
         <v>5066.5</v>
@@ -6617,19 +6504,19 @@
     </row>
     <row r="126" spans="1:12">
       <c r="A126" s="13"/>
-      <c r="B126" s="112" t="s">
-        <v>127</v>
-      </c>
-      <c r="C126" s="113"/>
-      <c r="D126" s="113"/>
-      <c r="E126" s="114"/>
+      <c r="B126" s="114" t="s">
+        <v>101</v>
+      </c>
+      <c r="C126" s="115"/>
+      <c r="D126" s="115"/>
+      <c r="E126" s="116"/>
       <c r="F126" s="6" t="s">
-        <v>172</v>
+        <v>145</v>
       </c>
       <c r="G126" s="7"/>
       <c r="H126" s="8"/>
       <c r="I126" s="76" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J126" s="5"/>
       <c r="K126" s="6"/>
@@ -6637,79 +6524,79 @@
     </row>
     <row r="127" spans="1:12">
       <c r="A127" s="13" t="s">
-        <v>173</v>
+        <v>146</v>
       </c>
       <c r="B127" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C127" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D127" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C127" s="27" t="s">
+      <c r="E127" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="D127" s="27" t="s">
+      <c r="F127" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="G127" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="E127" s="28" t="s">
+      <c r="H127" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="F127" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="G127" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="H127" s="28" t="s">
-        <v>86</v>
-      </c>
       <c r="I127" s="78" t="s">
-        <v>174</v>
+        <v>147</v>
       </c>
       <c r="J127" s="78" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="K127" s="31" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L127" s="28" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
     </row>
     <row r="128" spans="1:12">
       <c r="A128" s="40"/>
       <c r="B128" s="34" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="C128" s="35" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="D128" s="35" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="E128" s="36" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="F128" s="34" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="G128" s="35" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="H128" s="36" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="I128" s="79" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="J128" s="40"/>
       <c r="K128" s="34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L128" s="36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="129" spans="1:12" ht="15.75">
-      <c r="A129" s="115" t="s">
-        <v>175</v>
+      <c r="A129" s="112" t="s">
+        <v>148</v>
       </c>
       <c r="B129" s="43">
         <v>3091.5416666666665</v>
@@ -6746,8 +6633,8 @@
       </c>
     </row>
     <row r="130" spans="1:12" ht="15.75">
-      <c r="A130" s="116" t="s">
-        <v>176</v>
+      <c r="A130" s="113" t="s">
+        <v>149</v>
       </c>
       <c r="B130" s="60">
         <v>3934.625</v>

</xml_diff>

<commit_message>
One last fix to spreadsheets and did compare of all json's
</commit_message>
<xml_diff>
--- a/input/CodyRun/1/Std140_CE_b_Output.xlsx
+++ b/input/CodyRun/1/Std140_CE_b_Output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\JasonGlazer--ashrae-140-automation\input\CodyRun\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5D6735-FB03-4FDA-AB7A-7A311E29A4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB53585-C269-4014-ABE2-35424FAEC94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3570" yWindow="660" windowWidth="33600" windowHeight="20790" xr2:uid="{3967BC36-3351-4A62-97C9-7FE3A6239BBD}"/>
+    <workbookView xWindow="2490" yWindow="810" windowWidth="33600" windowHeight="20790" xr2:uid="{3967BC36-3351-4A62-97C9-7FE3A6239BBD}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -539,12 +539,6 @@
     <t>CE500</t>
   </si>
   <si>
-    <t>CE500 May-SCEp</t>
-  </si>
-  <si>
-    <t>CE510 May-SCEp</t>
-  </si>
-  <si>
     <t>CE520</t>
   </si>
   <si>
@@ -582,6 +576,12 @@
   </si>
   <si>
     <t xml:space="preserve">      C a s e   C E 5 3 0   A v e r a g e   D a i l y   O u t p u t s  -  f(ODB) sensitivity</t>
+  </si>
+  <si>
+    <t>CE500 May-Sep</t>
+  </si>
+  <si>
+    <t>CE510 May-Sep</t>
   </si>
 </sst>
 </file>
@@ -1524,8 +1524,8 @@
   </sheetPr>
   <dimension ref="A1:AR130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L138" sqref="L138"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1864,7 +1864,7 @@
       <c r="AB56" s="8"/>
       <c r="AC56" s="11"/>
       <c r="AD56" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="AE56" s="11"/>
       <c r="AF56" s="11"/>
@@ -1885,7 +1885,7 @@
       <c r="K57" s="15"/>
       <c r="L57" s="16"/>
       <c r="M57" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="N57" s="18"/>
       <c r="P57" s="13"/>
@@ -3012,7 +3012,7 @@
         <v>0.659418949771712</v>
       </c>
       <c r="P74" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="Q74" s="43">
         <v>10177</v>
@@ -3055,7 +3055,7 @@
     </row>
     <row r="75" spans="1:34" ht="15.75">
       <c r="A75" s="13" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="B75" s="53">
         <v>17434.537000000029</v>
@@ -3097,7 +3097,7 @@
         <v>0.5707216775598879</v>
       </c>
       <c r="P75" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="Q75" s="53">
         <v>11186</v>
@@ -3140,7 +3140,7 @@
     </row>
     <row r="76" spans="1:34" ht="15.75">
       <c r="A76" s="13" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="B76" s="53">
         <v>34848.63700000001</v>
@@ -3182,7 +3182,7 @@
         <v>0.57061546840956057</v>
       </c>
       <c r="P76" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="Q76" s="53">
         <v>11044</v>
@@ -3225,7 +3225,7 @@
     </row>
     <row r="77" spans="1:34" ht="15.75">
       <c r="A77" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B77" s="53">
         <v>25131.070000000262</v>
@@ -3267,7 +3267,7 @@
         <v>0.70226826484016935</v>
       </c>
       <c r="P77" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="Q77" s="53">
         <v>10639</v>
@@ -3310,7 +3310,7 @@
     </row>
     <row r="78" spans="1:34" ht="15.75">
       <c r="A78" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B78" s="53">
         <v>23619.743999999955</v>
@@ -3352,7 +3352,7 @@
         <v>0.68231392694061999</v>
       </c>
       <c r="P78" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="Q78" s="53">
         <v>9419</v>
@@ -3395,7 +3395,7 @@
     </row>
     <row r="79" spans="1:34" ht="15.75">
       <c r="A79" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B79" s="53">
         <v>20241.712999999996</v>
@@ -3437,7 +3437,7 @@
         <v>0.60138698630132004</v>
       </c>
       <c r="P79" s="13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="Q79" s="53">
         <v>7992</v>
@@ -3480,7 +3480,7 @@
     </row>
     <row r="80" spans="1:34" ht="15.75">
       <c r="A80" s="13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B80" s="71">
         <v>17442.46800000007</v>
@@ -3522,7 +3522,7 @@
         <v>0.41451598173521698</v>
       </c>
       <c r="P80" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Q80" s="53">
         <v>8846</v>
@@ -3565,7 +3565,7 @@
     </row>
     <row r="81" spans="1:44" ht="15.75">
       <c r="A81" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B81" s="53">
         <v>19536.572000000106</v>
@@ -3607,7 +3607,7 @@
         <v>0.40050913242005715</v>
       </c>
       <c r="P81" s="40" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q81" s="60">
         <v>7351</v>
@@ -3650,7 +3650,7 @@
     </row>
     <row r="82" spans="1:44" ht="15.75">
       <c r="A82" s="40" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B82" s="60">
         <v>15791.080999999982</v>
@@ -3698,7 +3698,7 @@
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
       <c r="E84" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
@@ -5225,7 +5225,7 @@
         <v>1.1329000000000001E-2</v>
       </c>
       <c r="P101" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="Q101" s="43">
         <v>4.1846218842416558</v>
@@ -5342,7 +5342,7 @@
         <v>1.1729E-2</v>
       </c>
       <c r="P102" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="Q102" s="53">
         <v>4.6895843211632684</v>
@@ -5459,7 +5459,7 @@
         <v>1.2378999999999999E-2</v>
       </c>
       <c r="P103" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="Q103" s="53">
         <v>3.8017291066282426</v>
@@ -5576,7 +5576,7 @@
         <v>1.4232E-2</v>
       </c>
       <c r="P104" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="Q104" s="53">
         <v>3.9857984589817197</v>
@@ -5692,7 +5692,7 @@
         <v>1.473E-2</v>
       </c>
       <c r="P105" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="Q105" s="53">
         <v>4.6380543633762521</v>
@@ -5808,7 +5808,7 @@
         <v>1.5684E-2</v>
       </c>
       <c r="P106" s="13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="Q106" s="71">
         <v>3.8400447427293063</v>
@@ -5924,7 +5924,7 @@
         <v>1.4539E-2</v>
       </c>
       <c r="P107" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Q107" s="71">
         <v>3.6666666666666665</v>
@@ -6040,7 +6040,7 @@
         <v>1.6878000000000001E-2</v>
       </c>
       <c r="P108" s="40" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q108" s="103">
         <v>4.1564885496183201</v>
@@ -6277,7 +6277,7 @@
     <row r="115" spans="1:12">
       <c r="A115" s="5"/>
       <c r="B115" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
@@ -6475,7 +6475,7 @@
     <row r="124" spans="1:12">
       <c r="A124" s="5"/>
       <c r="B124" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>

</xml_diff>